<commit_message>
added fake Expectation Maximization algorithm to Neural Networks) - sorry for adding whole netlab tree here, but it's dependency tree is really sick (and this lib... wtf it going on with passing almost everything by globals)
</commit_message>
<xml_diff>
--- a/6_semester/sterowanie_procesami_dyskretnymi/Lab4_PSFP_SimulatedAnealing/wyniki.xlsx
+++ b/6_semester/sterowanie_procesami_dyskretnymi/Lab4_PSFP_SimulatedAnealing/wyniki.xlsx
@@ -4679,8 +4679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
-      <selection activeCell="AH72" sqref="AH72"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q122" sqref="Q122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12102,8 +12102,8 @@
         <v>2.8381266908117528E-2</v>
       </c>
       <c r="Q122" s="2">
-        <f>AVERAGE(Q2:Q121)</f>
-        <v>4.3544192068927269E-3</v>
+        <f>_xlfn.STDEV.P(K2:O121)</f>
+        <v>1.8740450802975522E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>